<commit_message>
Quebra de linha e remoção de acentos da planilha
</commit_message>
<xml_diff>
--- a/perguntas/planilha.xlsx
+++ b/perguntas/planilha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fundacaougb-my.sharepoint.com/personal/2023121758_academicougb_com_br/Documents/Documentos/GitHub/JaguarIQ/perguntas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{6EE4EE0B-1399-4DF3-B913-54DFF7C3A10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE3B8CFB-D678-44EE-AD70-9570093EC146}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{6EE4EE0B-1399-4DF3-B913-54DFF7C3A10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F0CC58B-93DA-4680-8C6F-7895FC386C4D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,23 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="465">
   <si>
     <t>Hebraico, Latim e Grego</t>
   </si>
   <si>
-    <t>Lídia</t>
-  </si>
-  <si>
-    <t>Tércio</t>
-  </si>
-  <si>
-    <t>Teófilo</t>
-  </si>
-  <si>
-    <t>Júpiter e Mercúrio</t>
-  </si>
-  <si>
     <t>Matias</t>
   </si>
   <si>
@@ -71,24 +59,15 @@
     <t>Eliseu</t>
   </si>
   <si>
-    <t>Ágabo</t>
-  </si>
-  <si>
     <t>Campo de Sangue</t>
   </si>
   <si>
-    <t>Corpo, Alma e Espírito</t>
-  </si>
-  <si>
     <t>Tabita Dorcas</t>
   </si>
   <si>
     <t>Ao Deus Desconhecido</t>
   </si>
   <si>
-    <t>Saul, Davi e Salomão</t>
-  </si>
-  <si>
     <t>Formosa</t>
   </si>
   <si>
@@ -98,15 +77,6 @@
     <t>Sara</t>
   </si>
   <si>
-    <t>Concupiscência</t>
-  </si>
-  <si>
-    <t>Evangelico, Apostólico, Ensino, Pastoral e Profético</t>
-  </si>
-  <si>
-    <t>Sem, Cam e Jafé</t>
-  </si>
-  <si>
     <t>Laodiceia</t>
   </si>
   <si>
@@ -116,18 +86,12 @@
     <t>Carpideiras</t>
   </si>
   <si>
-    <t>Enéias</t>
-  </si>
-  <si>
     <t>Isaque</t>
   </si>
   <si>
     <t>Melquisedeque</t>
   </si>
   <si>
-    <t>Estevão</t>
-  </si>
-  <si>
     <t>Enoque</t>
   </si>
   <si>
@@ -146,39 +110,12 @@
     <t>Betume/Piche</t>
   </si>
   <si>
-    <t>Estáter</t>
-  </si>
-  <si>
-    <t>Moisés</t>
-  </si>
-  <si>
-    <t>Caifás</t>
-  </si>
-  <si>
-    <t>Betânia</t>
-  </si>
-  <si>
-    <t>Dídimo</t>
-  </si>
-  <si>
     <t>Saul</t>
   </si>
   <si>
     <t>Mestre</t>
   </si>
   <si>
-    <t>José de Arimateia</t>
-  </si>
-  <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Diná</t>
-  </si>
-  <si>
-    <t>Nazaré</t>
-  </si>
-  <si>
     <t>Lameque</t>
   </si>
   <si>
@@ -191,9 +128,6 @@
     <t>Bartolomeu</t>
   </si>
   <si>
-    <t>Isaías</t>
-  </si>
-  <si>
     <t>Tiago</t>
   </si>
   <si>
@@ -215,15 +149,9 @@
     <t>Jabal</t>
   </si>
   <si>
-    <t>Sansão</t>
-  </si>
-  <si>
     <t>Monte Carmelo</t>
   </si>
   <si>
-    <t>Fé, Graça, Escritura, Cristo e Glória a Deus</t>
-  </si>
-  <si>
     <t>Baruque</t>
   </si>
   <si>
@@ -233,45 +161,21 @@
     <t>Wittenberg</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantos foram os Cânticos de Salomão? </t>
-  </si>
-  <si>
     <t>Em quais idiomas foi escrito "Jesus Nazareno, o Rei dos Judeus" ?</t>
   </si>
   <si>
-    <t>Qual foi a primeira mulher convertida na Europa pelo apóstolo Paulo?</t>
-  </si>
-  <si>
     <t>Quem escreveu a carta de Paulo aos Romanos?</t>
   </si>
   <si>
     <t>A quem foi destinado o livro de Atos?</t>
   </si>
   <si>
-    <t>De quais planetas Paulo e Barnabé foram chamados?</t>
-  </si>
-  <si>
-    <t>Quem foi eleito apóstolo no lugar de Judas Iscariotes?</t>
-  </si>
-  <si>
-    <t>Quantos espias Josué enviou pra observar a terra?</t>
-  </si>
-  <si>
-    <t>Qual o nome do discípulo que orou para que Paulo recuperasse a visão?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onde os discípulos foram chamados de cristãos pela primeira vez? </t>
-  </si>
-  <si>
     <t>Quem foi o pai de todos os que tocam harpa e flauta?</t>
   </si>
   <si>
     <t>Quem fez o ferro do machado flutuar?</t>
   </si>
   <si>
-    <t>Qual o profeta que previu grande fome nos dias do imperador Romano Cláudio?</t>
-  </si>
-  <si>
     <t>O que significa Aceldama?</t>
   </si>
   <si>
@@ -281,33 +185,12 @@
     <t>Qual o nome da costureira que Pedro ressuscitou?</t>
   </si>
   <si>
-    <t>O que estava escrito no altar à Deus em Atenas?</t>
-  </si>
-  <si>
     <t>Quem foram os 3 primeiros reis de Israel?</t>
   </si>
   <si>
-    <t>Quantos anos Sansão julgou Israel?</t>
-  </si>
-  <si>
-    <t>Como se chamava a porta do templo onde os discípulos encontraram um coxo?</t>
-  </si>
-  <si>
     <t>Como se chamava o casal que morreu por ter mentido?</t>
   </si>
   <si>
-    <t>Qual é a única mulher cuja idade é mencionada na Bíblia?</t>
-  </si>
-  <si>
-    <t>De acordo com a Palavra de Deus qual é a raiz de todos os males</t>
-  </si>
-  <si>
-    <t>Quais sãos os 5 Ministérios?</t>
-  </si>
-  <si>
-    <t>Qual o nome dos 3 filhos de Noé?</t>
-  </si>
-  <si>
     <t>Qual igreja foi chamada de morna em Apocalipse?</t>
   </si>
   <si>
@@ -320,108 +203,39 @@
     <t xml:space="preserve">Qual o nome das mulheres contratadas para chorar e se lamentar? </t>
   </si>
   <si>
-    <t>Qual nome do paralítico que foi curado pela oração de Pedro em nome de Jesus ?</t>
-  </si>
-  <si>
-    <t>Qual o nome do filho de Abraão e Sara?</t>
-  </si>
-  <si>
-    <t>Qual o nome o Sacerdote rei de Salém a quem Abraão pagou o dízimo?</t>
-  </si>
-  <si>
-    <t>Qual nome do primeiro mártir da igreja ?</t>
-  </si>
-  <si>
-    <t>Quantos anos tinha Abraão quando nasceu Isaque ?</t>
-  </si>
-  <si>
-    <t>Quantas vezes ao todo o povo de Israel rodeou a cidade de Jericó?</t>
-  </si>
-  <si>
     <t>Andei 300 anos com Deus e depois sumi</t>
   </si>
   <si>
     <t>Quantos livros possui o Antigo Testamento?</t>
   </si>
   <si>
-    <t xml:space="preserve">Quem foi mãe de Zinrã, Jocsã, Medã, Midiã, Isbaque e Suá ? </t>
-  </si>
-  <si>
-    <t>Qual nome babilônico foi dado a Misael ?</t>
-  </si>
-  <si>
     <t>Qual profeta foi atolado na lama de uma cisterna ?</t>
   </si>
   <si>
-    <t xml:space="preserve">A mesa do rei me fez semelhante à todos. Quem sou eu ? </t>
-  </si>
-  <si>
-    <t>Qual material Noé usou para impermeabilização da Arca ?</t>
-  </si>
-  <si>
     <t>Qual moeda Pedro tirou da boca do peixe?</t>
   </si>
   <si>
-    <t>Quem a Bíblia afirma ter sido sepultado por Deus?</t>
-  </si>
-  <si>
-    <t>Como se chamava o doutor da lei que interrogou Jesus, e também Pedro e João?</t>
-  </si>
-  <si>
-    <t>A ascensão de Jesus aconteceu em qual cidade ?</t>
-  </si>
-  <si>
-    <t>Qual o apelido do apóstolo Tomé?</t>
-  </si>
-  <si>
     <t>Qual foi o primeiro Rei de Israel?</t>
   </si>
   <si>
     <t>O que significa Raboni?</t>
   </si>
   <si>
-    <t>Qual apóstolo ficou com Jesus ao pé da Cruz?</t>
-  </si>
-  <si>
-    <t>Qual era o nome da filha de Jacó ?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Em qual cidade as pessoas tentaram matar Jesus o jogando de um despenhadeiro? </t>
   </si>
   <si>
-    <t>Quem a Bíblia afirmou ser o homem mais manso da Terra ?</t>
-  </si>
-  <si>
-    <t>O centurião Cornélio fazia parte de qual corte?</t>
-  </si>
-  <si>
     <t>Em grego como fica o nome do rei Assuero?</t>
   </si>
   <si>
-    <t>Quem falou essa frase? "Pode vir alguma coisa boa de Nazaré ?"</t>
-  </si>
-  <si>
     <t>Qual foi o profeta que andou nu e descalço ?</t>
   </si>
   <si>
-    <t>Qual apóstolo foi morto a mando do rei Herodes ?</t>
-  </si>
-  <si>
-    <t>Qual profissão Neemias exercia no palácio do rei?</t>
-  </si>
-  <si>
     <t>Qual nome do homem que foi comandante do exercito do rei Davi?</t>
   </si>
   <si>
     <t>Qual nome do homem que foi comandante do exercito do rei Saul?</t>
   </si>
   <si>
-    <t>Em qual cidade Pedro teve a visão de um lençol que descia do céu cheio de animais ?</t>
-  </si>
-  <si>
-    <t>Qual nome da mãe de João Batista ?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quem foi o pai dos que habitam em tendas e possuem gado? </t>
   </si>
   <si>
@@ -431,21 +245,12 @@
     <t>Em que lugar o profeta Elias desafiou os 450 profetas de Baal ?</t>
   </si>
   <si>
-    <t>Quais são as "5 Solas"</t>
-  </si>
-  <si>
     <t>Quem começou a escrever o livro de Jeremias ?</t>
   </si>
   <si>
-    <t>Em qual dia, mês e ano, Martinho Lutero publicou suas 95 teses?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Na porta de qual igreja Martinho Lutero fixou as 95 teses ? </t>
   </si>
   <si>
-    <t>Qual foi o primeiro homem bígamo citado na Bíblia?</t>
-  </si>
-  <si>
     <t>Quem pediu o corpo de Jesus?</t>
   </si>
   <si>
@@ -467,60 +272,30 @@
     <t>Zacarias</t>
   </si>
   <si>
-    <t>Belém</t>
-  </si>
-  <si>
     <t>Gabriel</t>
   </si>
   <si>
-    <t>Ásia</t>
-  </si>
-  <si>
-    <t>Pérgamo</t>
-  </si>
-  <si>
-    <t>Midiã</t>
-  </si>
-  <si>
     <t>Meia-Noite</t>
   </si>
   <si>
-    <t>Pôncio Pilatos</t>
-  </si>
-  <si>
     <t>Silvano ou Silas</t>
   </si>
   <si>
-    <t>300 Denários</t>
-  </si>
-  <si>
-    <t>Ainoã e Abigail</t>
-  </si>
-  <si>
     <t>Malco</t>
   </si>
   <si>
-    <t>Sodoma, Gomorra, Admá e Zeboim</t>
-  </si>
-  <si>
     <t>Gaio</t>
   </si>
   <si>
     <t>Acazias</t>
   </si>
   <si>
-    <t>Irmãos</t>
-  </si>
-  <si>
     <t>Ismael</t>
   </si>
   <si>
     <t>Atos</t>
   </si>
   <si>
-    <t>9 da Manhã</t>
-  </si>
-  <si>
     <t>Herodes (Agripa I)</t>
   </si>
   <si>
@@ -530,9 +305,6 @@
     <t>Saulo</t>
   </si>
   <si>
-    <t>Abraão, Isaque e Jacó</t>
-  </si>
-  <si>
     <t>Candace</t>
   </si>
   <si>
@@ -548,9 +320,6 @@
     <t>Alexandre "Latoeiro"</t>
   </si>
   <si>
-    <t>Rãs</t>
-  </si>
-  <si>
     <t>Pentateuco</t>
   </si>
   <si>
@@ -572,30 +341,12 @@
     <t>Eli</t>
   </si>
   <si>
-    <t>Êutico</t>
-  </si>
-  <si>
     <t>Mateus e Lucas</t>
   </si>
   <si>
-    <t>Tértulo</t>
-  </si>
-  <si>
-    <t>Miriã</t>
-  </si>
-  <si>
-    <t>Públio</t>
-  </si>
-  <si>
     <t>Josebe-Bassebete</t>
   </si>
   <si>
-    <t>Moisés e Elias</t>
-  </si>
-  <si>
-    <t>Zípora</t>
-  </si>
-  <si>
     <t>Tiatira</t>
   </si>
   <si>
@@ -608,63 +359,30 @@
     <t>Lago de Fogo</t>
   </si>
   <si>
-    <t>(João) Marcos</t>
-  </si>
-  <si>
     <t>Marcos</t>
   </si>
   <si>
     <t>Figueira</t>
   </si>
   <si>
-    <t>Uzá</t>
-  </si>
-  <si>
     <t>Cirene</t>
   </si>
   <si>
-    <t>Labão</t>
-  </si>
-  <si>
-    <t>Jericó</t>
-  </si>
-  <si>
-    <t>Neustã</t>
-  </si>
-  <si>
-    <t>Icabô</t>
-  </si>
-  <si>
     <t>Elcana</t>
   </si>
   <si>
-    <t>Espírito Santo</t>
-  </si>
-  <si>
     <t>Jetro</t>
   </si>
   <si>
-    <t>Tiago e João</t>
-  </si>
-  <si>
     <t>Amarelo</t>
   </si>
   <si>
-    <t>Roboão</t>
-  </si>
-  <si>
     <t>Cam</t>
   </si>
   <si>
-    <t>Comer da árvore da vida</t>
-  </si>
-  <si>
     <t>Oseias</t>
   </si>
   <si>
-    <t>Arão e Hur</t>
-  </si>
-  <si>
     <t>Sangar</t>
   </si>
   <si>
@@ -683,45 +401,12 @@
     <t>Abede-Nego</t>
   </si>
   <si>
-    <t>José</t>
-  </si>
-  <si>
-    <t>Moriá</t>
-  </si>
-  <si>
-    <t>Dã</t>
-  </si>
-  <si>
-    <t>Benjamim e Judá</t>
-  </si>
-  <si>
     <t>Uzias</t>
   </si>
   <si>
-    <t>Recabe e Baaná</t>
-  </si>
-  <si>
-    <t>João e Tiago</t>
-  </si>
-  <si>
     <t>Himeneu e Alexandre</t>
   </si>
   <si>
-    <t>Aías</t>
-  </si>
-  <si>
-    <t>Pai, Filho e Espírito Santo</t>
-  </si>
-  <si>
-    <t>Nadabe e Abiú</t>
-  </si>
-  <si>
-    <t>Balaão</t>
-  </si>
-  <si>
-    <t>Absalão</t>
-  </si>
-  <si>
     <t>Fogo</t>
   </si>
   <si>
@@ -731,9 +416,6 @@
     <t>Malta</t>
   </si>
   <si>
-    <t>Trifena, Trifosa e Pérside</t>
-  </si>
-  <si>
     <t>Ester e Cantares</t>
   </si>
   <si>
@@ -743,15 +425,6 @@
     <t>He, La e Gr</t>
   </si>
   <si>
-    <t>Jônatas</t>
-  </si>
-  <si>
-    <t>Samá</t>
-  </si>
-  <si>
-    <t>Gólgota ou Calvário</t>
-  </si>
-  <si>
     <t>Bezalel</t>
   </si>
   <si>
@@ -761,9 +434,6 @@
     <t>Benjamim</t>
   </si>
   <si>
-    <t>Médico</t>
-  </si>
-  <si>
     <t>Mateus, Marcos e Lucas</t>
   </si>
   <si>
@@ -779,27 +449,18 @@
     <t>Ouro, prata, bronze, ferro e barro</t>
   </si>
   <si>
-    <t>César</t>
-  </si>
-  <si>
     <t>Sardes</t>
   </si>
   <si>
     <t>Petuel</t>
   </si>
   <si>
-    <t>João 11:35</t>
-  </si>
-  <si>
     <t>Arquipo</t>
   </si>
   <si>
     <t>Edom</t>
   </si>
   <si>
-    <t>Estêvão</t>
-  </si>
-  <si>
     <t>Morasti / Moresete</t>
   </si>
   <si>
@@ -815,18 +476,12 @@
     <t>Hananias</t>
   </si>
   <si>
-    <t>Hamã</t>
-  </si>
-  <si>
     <t>Filipe</t>
   </si>
   <si>
     <t>Piolhos</t>
   </si>
   <si>
-    <t>Simão</t>
-  </si>
-  <si>
     <t>Direita</t>
   </si>
   <si>
@@ -842,90 +497,48 @@
     <t>Jasom</t>
   </si>
   <si>
-    <t>Salomão</t>
-  </si>
-  <si>
     <t>Quem ouve a Palavra e a pratica</t>
   </si>
   <si>
     <t>Judas</t>
   </si>
   <si>
-    <t>maná</t>
-  </si>
-  <si>
     <t>Gamaliel</t>
   </si>
   <si>
-    <t>Jordão</t>
-  </si>
-  <si>
-    <t>Décimo Quinto</t>
-  </si>
-  <si>
     <t>Eliseba</t>
   </si>
   <si>
     <t>Patmos</t>
   </si>
   <si>
-    <t>Leão e urso</t>
-  </si>
-  <si>
     <t>Herodes</t>
   </si>
   <si>
     <t>Agar ou Hagar</t>
   </si>
   <si>
-    <t>Jesus é considerado Sumo Sacerdote segundo que ordem?</t>
-  </si>
-  <si>
     <t>Na casa de quem Paulo deixou sua capa?</t>
   </si>
   <si>
     <t>Qual significado do nome Melquisedeque?</t>
   </si>
   <si>
-    <t>Qual pessoa foi responsável por levar a oferta da Igreja de Filipos a Paulo?</t>
-  </si>
-  <si>
-    <t>Qual nome de um dos discípulos que iam no caminho de Emaús?</t>
-  </si>
-  <si>
     <t>Qual nome da mulher que foi escolhida pra cuidar de Davi na sua velhice?</t>
   </si>
   <si>
-    <t>Qual nome do sacerdote que ficou mudo por não acreditar num anjo do Senhor?</t>
-  </si>
-  <si>
     <t>Em qual cidade nasceu Jesus?</t>
   </si>
   <si>
     <t>Qual nome do ser celestial que anunciou o nascimento do segundo Elias?</t>
   </si>
   <si>
-    <t>A qual continente pertenciam às 7 igrejas do Apocalipse?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pra qual igreja foi destinada a terceira carta do Apocalipse? </t>
   </si>
   <si>
-    <t>O pai de Zípora era sacerdote de que região?</t>
-  </si>
-  <si>
-    <t>Em que horário aconteceu a décima praga?</t>
-  </si>
-  <si>
-    <t>Quem era governador da Judéia no 15º ano de Tibério César?</t>
-  </si>
-  <si>
     <t>Quem ajudou Pedro a escrever sua primeira carta?</t>
   </si>
   <si>
-    <t>Quanto valia o perfume derramado aos pés de Jesus em Betânia?</t>
-  </si>
-  <si>
     <t>Quem foi saqueado da cidade de Ziclague?</t>
   </si>
   <si>
@@ -935,153 +548,30 @@
     <t>Em que cidade Jesus foi ungido pra seu sepultamento?</t>
   </si>
   <si>
-    <t>Qual nome do soldado que teve a orelha cortada por um discípulo de Jesus?</t>
-  </si>
-  <si>
-    <t>Quais cidades foram destruídas pela ira de Deus?</t>
-  </si>
-  <si>
-    <t>A quem foi destinada a terceira carta de João?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “Acaso não há Deus em Israel?” Qual rei ouviu isso?</t>
-  </si>
-  <si>
-    <t>Qual parentesco de Jesus e Judas autor do penúltimo livro da Bíblia?</t>
-  </si>
-  <si>
-    <t>Quem um anjo revelou a sua mãe que sua mão seria contra todos?</t>
-  </si>
-  <si>
-    <t>Qual livro da Bíblia é uma continuação do 3 livro do novo testamento?</t>
-  </si>
-  <si>
-    <t>Mais de quantas fizeram voto de não comer e beber até que matassem o apostolo?</t>
-  </si>
-  <si>
-    <t>Em que horário aconteceu o Pentecostes?</t>
-  </si>
-  <si>
     <t>Com quantos anos Josias começou a reinar?</t>
   </si>
   <si>
-    <t>Quem presidiu o concílio de Jerusalém relatado em Atos?</t>
-  </si>
-  <si>
-    <t>O apóstolo Tiago foi morto a mandado de quem?</t>
-  </si>
-  <si>
-    <t>Quantos anos viveu o primeiro arrebatado na Bíblia?</t>
-  </si>
-  <si>
-    <t>O coxo que foi curado por Pedro e João tinha mais de quantos anos?</t>
-  </si>
-  <si>
-    <t>Quando foram apedrejar Estevão colocaram suas roupas aos pés de qual jovem?</t>
-  </si>
-  <si>
-    <t>Quantos dias Neemias demorou pra reconstruir os muros de Jerusalém?</t>
-  </si>
-  <si>
-    <t>Qual o nome dos 3 patriarcas da Nação de Israel?</t>
-  </si>
-  <si>
-    <t>Na época da Igreja Primitiva quem era a rainha da Etiópia?</t>
-  </si>
-  <si>
-    <t>Quanto tempo Moisés foi criado por seus pais antes de ser lançado no rio?</t>
-  </si>
-  <si>
-    <t>Quais mulheres aparecem na lista dos heróis da fé?</t>
-  </si>
-  <si>
-    <t>Quais árvores boas são citadas na parábola do Jotão?</t>
-  </si>
-  <si>
-    <t>Qual nome do fabricante de utensílios de lata que se opôs à Paulo?</t>
-  </si>
-  <si>
     <t>Qual foi a segunda praga das 10 pragas do Egito?</t>
   </si>
   <si>
-    <t>Como se chama o conjunto dos primeiros 5 livros da Bíblia?</t>
-  </si>
-  <si>
-    <t>Quem recebeu Pedro a porta depois que foi solto milagrosamente da prisão?</t>
-  </si>
-  <si>
-    <t>A descida do Espírito Santo se deu em qual festa judaica?</t>
-  </si>
-  <si>
     <t>Quem, por ter orado, Deus acrescentou-lhe mais 15 anos de vida ?</t>
   </si>
   <si>
     <t xml:space="preserve">Depois de ser ameaçado Elias se escondeu numa caverna em qual monte? </t>
   </si>
   <si>
-    <t xml:space="preserve">Qual nome da pessoa que morreu por não querer vender sua vinha ao rei? </t>
-  </si>
-  <si>
     <t>Quantas pedras Elias usou para edificar o altar no monte Carmelo?</t>
   </si>
   <si>
     <t>De quem eram filhos os homens que apanharam de um endemoniado?</t>
   </si>
   <si>
-    <t>Qual rei construiu o Túnel de Siloé?</t>
-  </si>
-  <si>
     <t>Qual sacerdote caiu da cadeira, quebrou o pescoço e morreu?</t>
   </si>
   <si>
-    <t>Quem morreu ao cair da janela enquanto o apóstolo aos gentios pregava?</t>
-  </si>
-  <si>
-    <t>Em quais livros está escrita a genealogia de Jesus?</t>
-  </si>
-  <si>
-    <t>Qual advogado apresentou a acusação de Paulo a Félix?</t>
-  </si>
-  <si>
-    <t>Qual o nome da irmã de Moisés?</t>
-  </si>
-  <si>
     <t>Quem era a principal autoridade da Ilha de Malta?</t>
   </si>
   <si>
-    <t>Quem era o líder do grupo dos 3 principais soldados de Davi?</t>
-  </si>
-  <si>
-    <t>Quais personagens do AT apareceram no Monte da Transfiguração?</t>
-  </si>
-  <si>
-    <t>Qual nome da esposa de Moisés?</t>
-  </si>
-  <si>
-    <t>Qual é a quarta igreja do Apocalipse?</t>
-  </si>
-  <si>
-    <t>Quantos receberam o Espírito Santo em Éfeso quando Paulo chegou lá?</t>
-  </si>
-  <si>
-    <t>Qual rainha que por não querer entrar na presença do rei foi substituída por Ester?</t>
-  </si>
-  <si>
-    <t>Qual nome da mãe de Salomão?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onde serão lançados o diabo, o falso profeta e a besta? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qual nome do jovem que desistiu de continuar com Paulo e Barnabé? </t>
-  </si>
-  <si>
-    <t>Quem que Paulo pediu pra Timoteo trazer consigo quando fosse visitá-lo?</t>
-  </si>
-  <si>
-    <t>Adão e Eva coseram folhas de que árvore para se cobrir depois da queda?</t>
-  </si>
-  <si>
     <t>Quem morreu por tentar segurar a Arca da Aliança?</t>
   </si>
   <si>
@@ -1094,349 +584,856 @@
     <t>O cego Bartimeu foi curado em qual cidade?</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantos anos viveu José do Egito? </t>
-  </si>
-  <si>
-    <t>Qual nome da serpente que Moisés levantou no deserto?</t>
-  </si>
-  <si>
-    <t>Qual nome uma criança recebeu quando Israel perdeu a Glória de Deus?</t>
-  </si>
-  <si>
     <t>Qual o nome do pai de Samuel?</t>
   </si>
   <si>
-    <t xml:space="preserve">As duas testemunhas do Apocalipse profetizarão por quantos dias? </t>
-  </si>
-  <si>
-    <t>Quem é o Paracleto que Jesus enviou?</t>
-  </si>
-  <si>
-    <t>Quem aconselhou Moises a repartir sua autoridade com outros líderes?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quais discípulos perguntaram a Jesus se podiam fazer descer fogo do céu? </t>
-  </si>
-  <si>
-    <t>Quantos anos tinha Arão quando foi falar com Faraó?</t>
-  </si>
-  <si>
     <t>O 4º selo do Apocalipse libera o cavalo de qual cor?</t>
   </si>
   <si>
     <t xml:space="preserve">Quantos versos tem o Salmo 119? </t>
   </si>
   <si>
-    <t>Qual era o nome da única filha de Lia?</t>
-  </si>
-  <si>
     <t>No reinado de qual rei Israel foi dividida em Reino do Norte e Reino do Sul?</t>
   </si>
   <si>
     <t>Qual filho foi amaldiçoado por expor a nudez de seu pai?</t>
   </si>
   <si>
-    <t>Qual recompensa foi dada aos vencedores da Igreja de Éfeso?</t>
-  </si>
-  <si>
     <t>Qual profeta se casou com uma prostituta?</t>
   </si>
   <si>
-    <t>Quais pessoas seguravam as mão de Moisés enquanto Israel lutava?</t>
-  </si>
-  <si>
     <t>Quem matou 600 Filisteus com uma aguilhada de bois?</t>
   </si>
   <si>
-    <t>Tiago e João perguntaram a Jesus para que mandassem fogo aonde?</t>
-  </si>
-  <si>
-    <t>Em quais idiomas a Bíblia foi escrita?</t>
-  </si>
-  <si>
     <t>A quem Neco matou em Megido?</t>
   </si>
   <si>
-    <t>Em Romanos 16:12 Paulo envia saudação a quais duas mulheres?</t>
-  </si>
-  <si>
-    <t>Após orar a Deus Ezequias teve a vida prolongada por quantos anos?</t>
-  </si>
-  <si>
-    <t>Qual nome Azarias recebeu na Babilônia?</t>
-  </si>
-  <si>
-    <t>Qual o nome de Barnabé?</t>
-  </si>
-  <si>
-    <t>Qual nome do monte onde Abraão ofereceu seu filho como oferta?</t>
-  </si>
-  <si>
     <t>De qual tribo era Aoliabe?</t>
   </si>
   <si>
     <t>Quais tribos formavam o Reino do Sul?</t>
   </si>
   <si>
-    <t>No ano da morte de qual rei, Isaias teve a visão do seu chamado?</t>
-  </si>
-  <si>
-    <t>Quais os 2 irmãos que tiveram suas mãos e pés decepados?</t>
-  </si>
-  <si>
-    <t>Quantos anos viveu o homem mais velho mencionado na Bíblia?</t>
-  </si>
-  <si>
     <t>A quem Jesus chamou de Boanerges?</t>
   </si>
   <si>
-    <t>Quais pessoas Paulo entregou a satanás para serem castigados?</t>
-  </si>
-  <si>
     <t>Qual profeta rasgou a capa na frente de um rei em 12 partes?</t>
   </si>
   <si>
     <t>O Batismo dos que Creem e ser imergido no.....</t>
   </si>
   <si>
-    <t>Quais irmãos morreram por levarem fogo estranho para o tabernáculo?</t>
-  </si>
-  <si>
-    <t>Qual o cavaleiro que teve o seu pé imprensado contra o muro?</t>
-  </si>
-  <si>
     <t>Quem tinha um cabelo que pesava mais de 2 quilos?</t>
   </si>
   <si>
-    <t>Quando recebemos uma convicção interna de que a Palavra é a verdade?</t>
-  </si>
-  <si>
-    <t>Quem escreveu o livro de Atos dos Apóstolos?</t>
-  </si>
-  <si>
-    <t>Qual nome da Ilha onde Paulo teve a mão mordida por uma víbora?</t>
-  </si>
-  <si>
-    <t>Quem são as 3 mulheres ditas por Paulo que muito trabalharam?</t>
-  </si>
-  <si>
-    <t>Em quais livros da Bíblia não aparece a palavra Deus?</t>
-  </si>
-  <si>
-    <t>Qual nome da bisavó de Davi?</t>
-  </si>
-  <si>
-    <t>Quantos profetas de Aserá comiam da mesa de Jezabel?</t>
-  </si>
-  <si>
-    <t>Quem matou um gigante que tinha 6 dedos nas mãos e nos pés?</t>
-  </si>
-  <si>
     <t>Qual guerreiro ficou famoso por defender um campo de lentilha?</t>
   </si>
   <si>
     <t>Qual nome do monte onde Jesus foi crucificado?</t>
   </si>
   <si>
-    <t>Quantos espias Josué enviou para observar a Terra?</t>
-  </si>
-  <si>
-    <t>Qual foi a primeira pessoa que a Bíblia relata ter sido cheia do Espírito Santo para um fim específico?</t>
-  </si>
-  <si>
-    <t>As margens de qual rio Ezequiel teve a visão dos 4 seres viventes?</t>
-  </si>
-  <si>
-    <t>O apóstolo Paulo era natural de qual tribo de Israel?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qual profissão do escritor do livro de Atos? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quem recusou ser chamado de filho da filha de Faraó? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quais são os evangelhos sinóticos? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantos anos tinha Noé quando as águas do dilúvio inundaram a terra? </t>
-  </si>
-  <si>
-    <t>Na queda de Satanás descrita no livro de Ezequiel, ele(Satanás) é comparado ao Rei de qual cidade?</t>
-  </si>
-  <si>
-    <t>De qual local Moisés avistou a Terra Prometida?</t>
-  </si>
-  <si>
     <t>Qual nome da mulher que aceitou esconder seu inimigo, deu-lhe um copo de leite mas depois o matou com uma estaca e martelo?</t>
   </si>
   <si>
-    <t>De quais matérias era formada a estátua do sonho de Nabucodonosor?</t>
-  </si>
-  <si>
-    <t>Qual nome do pai de João Batista?</t>
-  </si>
-  <si>
-    <t>A quem Paulo apelou em seu último julgamento antes de ir para Roma?</t>
-  </si>
-  <si>
     <t>Qual foi a Igreja que Jesus afirmou ter fama de estar viva mas na verdade estava morta?</t>
   </si>
   <si>
-    <t>Qual era a altura(em côvados) da estátua de ouro que Nabucodonosor mandou fazer pra si?</t>
-  </si>
-  <si>
     <t>Qual o nome do pai do profeta Joel?</t>
   </si>
   <si>
     <t>Qual o nome da cidade fundada por Caim, depois que saiu da presença de Deus ?</t>
   </si>
   <si>
-    <t>Qual é o menor versículo da Bíblia sagrada?</t>
-  </si>
-  <si>
     <t>A quem Paulo chamou de “meu companheiro de lutas”?</t>
   </si>
   <si>
     <t>A quem foi destinada a profecia de Obadias?</t>
   </si>
   <si>
-    <t>Qual foi o primeiro mártir da igreja ?</t>
-  </si>
-  <si>
-    <t>Miquéias era natural de qual cidade?</t>
-  </si>
-  <si>
-    <t>De qual reino era o homem que deu a notícia da morte de Absalão a Davi?</t>
-  </si>
-  <si>
-    <t>Qual nome da mãe do profeta Samuel?</t>
-  </si>
-  <si>
-    <t>Por quantas moedas José foi vendido pelo seus irmãos?</t>
-  </si>
-  <si>
     <t>Quanto rapazes foram comidos por 2 ursas por zombarem do profeta?</t>
   </si>
   <si>
-    <t xml:space="preserve">Quem escreveu o livro de Levítico? </t>
-  </si>
-  <si>
-    <t>Quem reconstruiu os muros de Jericó a custa da vida de seus filhos?</t>
-  </si>
-  <si>
     <t>Qual verdadeiro nome de Sadraque?</t>
   </si>
   <si>
-    <t>Quem foi enforcado na sua própria forca?</t>
-  </si>
-  <si>
-    <t>Quantos dias levaram pra embalsamar o corpo de Jacó?</t>
-  </si>
-  <si>
-    <t>Após a morte de Estêvão quem vai para Samaria pregar o Evangelho?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qual das 10 pragas os magos do Egito não puderam replicar? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quem ofereceu dinheiro aos apóstolos para ter o poder de orar e as pessoas receberem o Espírito Santo? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Qual nome da rua que Deus mandou Ananias ir para encontrar Saulo? </t>
   </si>
   <si>
-    <t xml:space="preserve">Qual rei foi usado por Deus para devolver os utensílios sagrados que Nabucodonosor havia roubado do Templo do Senhor? </t>
-  </si>
-  <si>
-    <t>Qual era o nome babilônico de Daniel?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qual nome do filho primogênito de Davi? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qual era a idade de Calebe quando pediu Hebrom para Josué? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantos capítulos tem o livro de Naum? </t>
-  </si>
-  <si>
-    <t>Quem recebeu Paulo e Silas em sua casa em Tessalônica e por conta disso foi interrogado?</t>
-  </si>
-  <si>
-    <t>Quais discípulos perguntaram a Jesus se podiam fazer descer fogo do céu?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adão viveu quantos anos? </t>
-  </si>
-  <si>
-    <t>Quantos capítulos tem o Novo Testamento?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quem escreveu Eclesiastes? </t>
   </si>
   <si>
-    <t>Quem Jesus afirmou ser seu pai e mãe em Lc 8?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Na casa de quem Paulo estava quando Ananias foi ao seu encontro? </t>
   </si>
   <si>
-    <t xml:space="preserve">Quantos anciãos receberam do Espírito que estava sobre Moisés? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Quais objetos foram colocados na arca da aliança? </t>
   </si>
   <si>
-    <t>Qual igreja habitava onde estava o trono de Satanás?</t>
-  </si>
-  <si>
-    <t>Paulo foi criado aos pés de qual rabi?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paulo e Barnabé foram chamados de quais planetas? </t>
-  </si>
-  <si>
     <t>Em qual rio Jesus foi batizado?</t>
   </si>
   <si>
-    <t xml:space="preserve">Quais livros da Bíblia narram o nascimento de Jesus? </t>
-  </si>
-  <si>
     <t>Qual profeta foi zombado por ser calvo?</t>
   </si>
   <si>
-    <t>Em qual ano do império de Tibério César, João Batista começou a pregar no deserto?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como se chamava a mulher de Arão? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Por quantas vezes o povo de Israel rodeou a cidade de Jericó? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quem morreu durante uma pregação de Paulo? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Qual rei cujo corpo foi afixado no muro de uma cidade? </t>
   </si>
   <si>
-    <t>Qual o nome da ilha onde João escreveu o livro de Apocalipse?</t>
-  </si>
-  <si>
-    <t>Quantas pessoas morreram com a queda da Torre de Siloé?</t>
-  </si>
-  <si>
     <t>Quais animais Davi matou pra proteger suas ovelhas?</t>
   </si>
   <si>
-    <t>Quem foi comido de bicho por não glorificar a Deus?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quem era a mãe de Ismael, filho de Abraão? </t>
-  </si>
-  <si>
     <t>Quem encontrou um reino quando procurava umas jumentas pertencentes ao seu pai?</t>
+  </si>
+  <si>
+    <t>Saul, Davi e Salomao</t>
+  </si>
+  <si>
+    <t>Quantos anos Sansao julgou Israel?</t>
+  </si>
+  <si>
+    <t>Qual o nome do filho de Abraao e Sara?</t>
+  </si>
+  <si>
+    <t>Estevao</t>
+  </si>
+  <si>
+    <t>Quantos anos tinha Abraao quando nasceu Isaque ?</t>
+  </si>
+  <si>
+    <t>A ascensao de Jesus aconteceu em qual cidade ?</t>
+  </si>
+  <si>
+    <t>Joao</t>
+  </si>
+  <si>
+    <t>Qual nome da mae de Joao Batista ?</t>
+  </si>
+  <si>
+    <t>Sansao</t>
+  </si>
+  <si>
+    <t>Quais sao as "5 Solas"</t>
+  </si>
+  <si>
+    <t>Qual nome do sacerdote que ficou mudo por nao acreditar num anjo do Senhor?</t>
+  </si>
+  <si>
+    <t>Midia</t>
+  </si>
+  <si>
+    <t>Ainoa e Abigail</t>
+  </si>
+  <si>
+    <t>A quem foi destinada a terceira carta de Joao?</t>
+  </si>
+  <si>
+    <t>Irmaos</t>
+  </si>
+  <si>
+    <t>Quem um anjo revelou a sua mae que sua mao seria contra todos?</t>
+  </si>
+  <si>
+    <t>9 da Manha</t>
+  </si>
+  <si>
+    <t>O coxo que foi curado por Pedro e Joao tinha mais de quantos anos?</t>
+  </si>
+  <si>
+    <t>Qual o nome dos 3 patriarcas da Naçao de Israel?</t>
+  </si>
+  <si>
+    <t>Ras</t>
+  </si>
+  <si>
+    <t>Quem recebeu Pedro a porta depois que foi solto milagrosamente da prisao?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual nome da pessoa que morreu por nao querer vender sua vinha ao rei? </t>
+  </si>
+  <si>
+    <t>Miria</t>
+  </si>
+  <si>
+    <t>Quais personagens do AT apareceram no Monte da Transfiguraçao?</t>
+  </si>
+  <si>
+    <t>Qual nome da mae de Salomao?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onde serao lançados o diabo, o falso profeta e a besta? </t>
+  </si>
+  <si>
+    <t>(Joao) Marcos</t>
+  </si>
+  <si>
+    <t>Labao</t>
+  </si>
+  <si>
+    <t>Neusta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As duas testemunhas do Apocalipse profetizarao por quantos dias? </t>
+  </si>
+  <si>
+    <t>Tiago e Joao</t>
+  </si>
+  <si>
+    <t>Roboao</t>
+  </si>
+  <si>
+    <t>Arao e Hur</t>
+  </si>
+  <si>
+    <t>Tiago e Joao perguntaram a Jesus para que mandassem fogo aonde?</t>
+  </si>
+  <si>
+    <t>Em Romanos 16:12 Paulo envia saudaçao a quais duas mulheres?</t>
+  </si>
+  <si>
+    <t>Qual nome do monte onde Abraao ofereceu seu filho como oferta?</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>No ano da morte de qual rei, Isaias teve a visao do seu chamado?</t>
+  </si>
+  <si>
+    <t>Joao e Tiago</t>
+  </si>
+  <si>
+    <t>Balaao</t>
+  </si>
+  <si>
+    <t>Absalao</t>
+  </si>
+  <si>
+    <t>Quem sao as 3 mulheres ditas por Paulo que muito trabalharam?</t>
+  </si>
+  <si>
+    <t>As margens de qual rio Ezequiel teve a visao dos 4 seres viventes?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual profissao do escritor do livro de Atos? </t>
+  </si>
+  <si>
+    <t>Qual nome do pai de Joao Batista?</t>
+  </si>
+  <si>
+    <t>Joao 11:35</t>
+  </si>
+  <si>
+    <t>Qual nome da mae do profeta Samuel?</t>
+  </si>
+  <si>
+    <t>Hama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual das 10 pragas os magos do Egito nao puderam replicar? </t>
+  </si>
+  <si>
+    <t>Simao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adao viveu quantos anos? </t>
+  </si>
+  <si>
+    <t>Salomao</t>
+  </si>
+  <si>
+    <t>Quem Jesus afirmou ser seu pai e mae em Lc 8?</t>
+  </si>
+  <si>
+    <t>Jordao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como se chamava a mulher de Arao? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quem morreu durante uma pregaçao de Paulo? </t>
+  </si>
+  <si>
+    <t>Qual o nome da ilha onde Joao escreveu o livro de Apocalipse?</t>
+  </si>
+  <si>
+    <t>Leao e urso</t>
+  </si>
+  <si>
+    <t>Quem foi comido de bicho por nao glorificar a Deus?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quem era a mae de Ismael, filho de Abraao? </t>
+  </si>
+  <si>
+    <t>O que estava escrito no altar a Deus em Atenas?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A mesa do rei me fez semelhante a todos. Quem sou eu ? </t>
+  </si>
+  <si>
+    <t>A qual continente pertenciam as 7 igrejas do Apocalipse?</t>
+  </si>
+  <si>
+    <t>Qual o profeta que previu grande fome nos dias do imperador Romano Claudio?</t>
+  </si>
+  <si>
+    <t>agabo</t>
+  </si>
+  <si>
+    <t>Qual nome do primeiro martir da igreja ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quem foi mae de Zinra, Jocsa, Meda, Midia, Isbaque e Sua ? </t>
+  </si>
+  <si>
+    <t>Estater</t>
+  </si>
+  <si>
+    <t>Caifas</t>
+  </si>
+  <si>
+    <t>Dina</t>
+  </si>
+  <si>
+    <t>Qual profissao Neemias exercia no palacio do rei?</t>
+  </si>
+  <si>
+    <t>Qual pessoa foi responsavel por levar a oferta da Igreja de Filipos a Paulo?</t>
+  </si>
+  <si>
+    <t>asia</t>
+  </si>
+  <si>
+    <t>300 Denarios</t>
+  </si>
+  <si>
+    <t>Sodoma, Gomorra, Adma e Zeboim</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> “Acaso nao ha Deus em Israel?” Qual rei ouviu isso?</t>
+  </si>
+  <si>
+    <t>Em que horario aconteceu o Pentecostes?</t>
+  </si>
+  <si>
+    <t>Quais arvores boas sao citadas na parabola do Jotao?</t>
+  </si>
+  <si>
+    <t>Em quais livros esta escrita a genealogia de Jesus?</t>
+  </si>
+  <si>
+    <t>Quem que Paulo pediu pra Timoteo trazer consigo quando fosse visita-lo?</t>
+  </si>
+  <si>
+    <t>Adao e Eva coseram folhas de que arvore para se cobrir depois da queda?</t>
+  </si>
+  <si>
+    <t>Uza</t>
+  </si>
+  <si>
+    <t>Comer da arvore da vida</t>
+  </si>
+  <si>
+    <t>Moria</t>
+  </si>
+  <si>
+    <t>Benjamim e Juda</t>
+  </si>
+  <si>
+    <t>Recabe e Baana</t>
+  </si>
+  <si>
+    <t>Quais pessoas Paulo entregou a satanas para serem castigados?</t>
+  </si>
+  <si>
+    <t>Quais irmaos morreram por levarem fogo estranho para o tabernaculo?</t>
+  </si>
+  <si>
+    <t>Quantos profetas de Asera comiam da mesa de Jezabel?</t>
+  </si>
+  <si>
+    <t>Sama</t>
+  </si>
+  <si>
+    <t>Qual foi o primeiro martir da igreja ?</t>
+  </si>
+  <si>
+    <t>mana</t>
+  </si>
+  <si>
+    <t>Qual igreja habitava onde estava o trono de Satanas?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantos foram os Canticos de Salomao? </t>
+  </si>
+  <si>
+    <t>Betania</t>
+  </si>
+  <si>
+    <t>Concupiscencia</t>
+  </si>
+  <si>
+    <t>Em qual dia, mes e ano, Martinho Lutero publicou suas 95 teses?</t>
+  </si>
+  <si>
+    <t>eutico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual nome do filho primogenito de Davi? </t>
+  </si>
+  <si>
+    <t>Tercio</t>
+  </si>
+  <si>
+    <t>De quais planetas Paulo e Barnabe foram chamados?</t>
+  </si>
+  <si>
+    <t>Quantos espias Josue enviou pra observar a terra?</t>
+  </si>
+  <si>
+    <t>De acordo com a Palavra de Deus qual e a raiz de todos os males</t>
+  </si>
+  <si>
+    <t>Quais saos os 5 Ministerios?</t>
+  </si>
+  <si>
+    <t>Qual o nome dos 3 filhos de Noe?</t>
+  </si>
+  <si>
+    <t>Sem, Cam e Jafe</t>
+  </si>
+  <si>
+    <t>Eneias</t>
+  </si>
+  <si>
+    <t>Qual material Noe usou para impermeabilizaçao da Arca ?</t>
+  </si>
+  <si>
+    <t>Moises</t>
+  </si>
+  <si>
+    <t>Como se chamava o doutor da lei que interrogou Jesus, e tambem Pedro e Joao?</t>
+  </si>
+  <si>
+    <t>Jose de Arimateia</t>
+  </si>
+  <si>
+    <t>Nazare</t>
+  </si>
+  <si>
+    <t>O centuriao Cornelio fazia parte de qual corte?</t>
+  </si>
+  <si>
+    <t>Quem falou essa frase? "Pode vir alguma coisa boa de Nazare ?"</t>
+  </si>
+  <si>
+    <t>Em qual cidade Pedro teve a visao de um lençol que descia do ceu cheio de animais ?</t>
+  </si>
+  <si>
+    <t>Jesus e considerado Sumo Sacerdote segundo que ordem?</t>
+  </si>
+  <si>
+    <t>Belem</t>
+  </si>
+  <si>
+    <t>Pergamo</t>
+  </si>
+  <si>
+    <t>Em que horario aconteceu a decima praga?</t>
+  </si>
+  <si>
+    <t>Quem era governador da Judeia no 15º ano de Tiberio Cesar?</t>
+  </si>
+  <si>
+    <t>Quanto valia o perfume derramado aos pes de Jesus em Betania?</t>
+  </si>
+  <si>
+    <t>Mais de quantas fizeram voto de nao comer e beber ate que matassem o apostolo?</t>
+  </si>
+  <si>
+    <t>Quando foram apedrejar Estevao colocaram suas roupas aos pes de qual jovem?</t>
+  </si>
+  <si>
+    <t>Quantos dias Neemias demorou pra reconstruir os muros de Jerusalem?</t>
+  </si>
+  <si>
+    <t>Quanto tempo Moises foi criado por seus pais antes de ser lançado no rio?</t>
+  </si>
+  <si>
+    <t>Qual advogado apresentou a acusaçao de Paulo a Felix?</t>
+  </si>
+  <si>
+    <t>Tertulo</t>
+  </si>
+  <si>
+    <t>Qual o nome da irma de Moises?</t>
+  </si>
+  <si>
+    <t>Moises e Elias</t>
+  </si>
+  <si>
+    <t>Qual nome da esposa de Moises?</t>
+  </si>
+  <si>
+    <t>Qual e a quarta igreja do Apocalipse?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual nome do jovem que desistiu de continuar com Paulo e Barnabe? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantos anos viveu Jose do Egito? </t>
+  </si>
+  <si>
+    <t>Qual nome da serpente que Moises levantou no deserto?</t>
+  </si>
+  <si>
+    <t>Quem e o Paracleto que Jesus enviou?</t>
+  </si>
+  <si>
+    <t>Qual recompensa foi dada aos vencedores da Igreja de efeso?</t>
+  </si>
+  <si>
+    <t>Quais pessoas seguravam as mao de Moises enquanto Israel lutava?</t>
+  </si>
+  <si>
+    <t>Qual o nome de Barnabe?</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Quais os 2 irmaos que tiveram suas maos e pes decepados?</t>
+  </si>
+  <si>
+    <t>Qual o cavaleiro que teve o seu pe imprensado contra o muro?</t>
+  </si>
+  <si>
+    <t>Quando recebemos uma convicçao interna de que a Palavra e a verdade?</t>
+  </si>
+  <si>
+    <t>Trifena, Trifosa e Perside</t>
+  </si>
+  <si>
+    <t>Quem matou um gigante que tinha 6 dedos nas maos e nos pes?</t>
+  </si>
+  <si>
+    <t>Quantos espias Josue enviou para observar a Terra?</t>
+  </si>
+  <si>
+    <t>Medico</t>
+  </si>
+  <si>
+    <t>Na queda de Satanas descrita no livro de Ezequiel, ele(Satanas) e comparado ao Rei de qual cidade?</t>
+  </si>
+  <si>
+    <t>De qual local Moises avistou a Terra Prometida?</t>
+  </si>
+  <si>
+    <t>De quais materias era formada a estatua do sonho de Nabucodonosor?</t>
+  </si>
+  <si>
+    <t>Cesar</t>
+  </si>
+  <si>
+    <t>Miqueias era natural de qual cidade?</t>
+  </si>
+  <si>
+    <t>Por quantas moedas Jose foi vendido pelo seus irmaos?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual era a idade de Calebe quando pediu Hebrom para Josue? </t>
+  </si>
+  <si>
+    <t>Paulo foi criado aos pes de qual rabi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paulo e Barnabe foram chamados de quais planetas? </t>
+  </si>
+  <si>
+    <t>Em qual ano do imperio de Tiberio Cesar, Joao Batista começou a pregar no deserto?</t>
+  </si>
+  <si>
+    <t>Decimo Quinto</t>
+  </si>
+  <si>
+    <t>Quantas pessoas morreram com a queda da Torre de Siloe?</t>
+  </si>
+  <si>
+    <t>Lidia</t>
+  </si>
+  <si>
+    <t>Qual o nome do discipulo que orou para que Paulo recuperasse a visao?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onde os discipulos foram chamados de cristaos pela primeira vez? </t>
+  </si>
+  <si>
+    <t>Corpo, Alma e Espirito</t>
+  </si>
+  <si>
+    <t>Como se chamava a porta do templo onde os discipulos encontraram um coxo?</t>
+  </si>
+  <si>
+    <t>Qual nome do paralitico que foi curado pela oraçao de Pedro em nome de Jesus ?</t>
+  </si>
+  <si>
+    <t>Qual o nome o Sacerdote rei de Salem a quem Abraao pagou o dizimo?</t>
+  </si>
+  <si>
+    <t>Quem a Biblia afirma ter sido sepultado por Deus?</t>
+  </si>
+  <si>
+    <t>Didimo</t>
+  </si>
+  <si>
+    <t>Quem a Biblia afirmou ser o homem mais manso da Terra ?</t>
+  </si>
+  <si>
+    <t>Qual foi o primeiro homem bigamo citado na Biblia?</t>
+  </si>
+  <si>
+    <t>Isaias</t>
+  </si>
+  <si>
+    <t>O pai de Zipora era sacerdote de que regiao?</t>
+  </si>
+  <si>
+    <t>Qual nome do soldado que teve a orelha cortada por um discipulo de Jesus?</t>
+  </si>
+  <si>
+    <t>Quais cidades foram destruidas pela ira de Deus?</t>
+  </si>
+  <si>
+    <t>Qual livro da Biblia e uma continuaçao do 3 livro do novo testamento?</t>
+  </si>
+  <si>
+    <t>Quem presidiu o concilio de Jerusalem relatado em Atos?</t>
+  </si>
+  <si>
+    <t>Quantos anos viveu o primeiro arrebatado na Biblia?</t>
+  </si>
+  <si>
+    <t>Como se chama o conjunto dos primeiros 5 livros da Biblia?</t>
+  </si>
+  <si>
+    <t>A descida do Espirito Santo se deu em qual festa judaica?</t>
+  </si>
+  <si>
+    <t>Quem era o lider do grupo dos 3 principais soldados de Davi?</t>
+  </si>
+  <si>
+    <t>Zipora</t>
+  </si>
+  <si>
+    <t>Quantos receberam o Espirito Santo em efeso quando Paulo chegou la?</t>
+  </si>
+  <si>
+    <t>Qual rainha que por nao querer entrar na presença do rei foi substituida por Ester?</t>
+  </si>
+  <si>
+    <t>Espirito Santo</t>
+  </si>
+  <si>
+    <t>Quem aconselhou Moises a repartir sua autoridade com outros lideres?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quais discipulos perguntaram a Jesus se podiam fazer descer fogo do ceu? </t>
+  </si>
+  <si>
+    <t>Em quais idiomas a Biblia foi escrita?</t>
+  </si>
+  <si>
+    <t>Quantos anos viveu o homem mais velho mencionado na Biblia?</t>
+  </si>
+  <si>
+    <t>Aias</t>
+  </si>
+  <si>
+    <t>Pai, Filho e Espirito Santo</t>
+  </si>
+  <si>
+    <t>Qual nome da Ilha onde Paulo teve a mao mordida por uma vibora?</t>
+  </si>
+  <si>
+    <t>Em quais livros da Biblia nao aparece a palavra Deus?</t>
+  </si>
+  <si>
+    <t>Qual foi a primeira pessoa que a Biblia relata ter sido cheia do Espirito Santo para um fim especifico?</t>
+  </si>
+  <si>
+    <t>Qual e o menor versiculo da Biblia sagrada?</t>
+  </si>
+  <si>
+    <t>De qual reino era o homem que deu a noticia da morte de Absalao a Davi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quem escreveu o livro de Levitico? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual rei foi usado por Deus para devolver os utensilios sagrados que Nabucodonosor havia roubado do Templo do Senhor? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantos capitulos tem o livro de Naum? </t>
+  </si>
+  <si>
+    <t>Quais discipulos perguntaram a Jesus se podiam fazer descer fogo do ceu?</t>
+  </si>
+  <si>
+    <t>Quantos capitulos tem o Novo Testamento?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantos anciaos receberam do Espirito que estava sobre Moises? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quais livros da Biblia narram o nascimento de Jesus? </t>
+  </si>
+  <si>
+    <t>Qual nome babilonico foi dado a Misael ?</t>
+  </si>
+  <si>
+    <t>Poncio Pilatos</t>
+  </si>
+  <si>
+    <t>Qual nome do fabricante de utensilios de lata que se opos a Paulo?</t>
+  </si>
+  <si>
+    <t>Icabo</t>
+  </si>
+  <si>
+    <t>Qual nome Azarias recebeu na Babilonia?</t>
+  </si>
+  <si>
+    <t>Jonatas</t>
+  </si>
+  <si>
+    <t>Qual era a altura(em covados) da estatua de ouro que Nabucodonosor mandou fazer pra si?</t>
+  </si>
+  <si>
+    <t>Qual era o nome babilonico de Daniel?</t>
+  </si>
+  <si>
+    <t>Quem recebeu Paulo e Silas em sua casa em Tessalonica e por conta disso foi interrogado?</t>
+  </si>
+  <si>
+    <t>Qual foi a primeira mulher convertida na Europa pelo apostolo Paulo?</t>
+  </si>
+  <si>
+    <t>Teofilo</t>
+  </si>
+  <si>
+    <t>Quem foi eleito apostolo no lugar de Judas Iscariotes?</t>
+  </si>
+  <si>
+    <t>Evangelico, Apostolico, Ensino, Pastoral e Profetico</t>
+  </si>
+  <si>
+    <t>Quantas vezes ao todo o povo de Israel rodeou a cidade de Jerico?</t>
+  </si>
+  <si>
+    <t>Qual o apelido do apostolo Tome?</t>
+  </si>
+  <si>
+    <t>Qual apostolo ficou com Jesus ao pe da Cruz?</t>
+  </si>
+  <si>
+    <t>Qual era o nome da filha de Jaco ?</t>
+  </si>
+  <si>
+    <t>Qual apostolo foi morto a mando do rei Herodes ?</t>
+  </si>
+  <si>
+    <t>Fe, Graça, Escritura, Cristo e Gloria a Deus</t>
+  </si>
+  <si>
+    <t>O apostolo Tiago foi morto a mandado de quem?</t>
+  </si>
+  <si>
+    <t>Abraao, Isaque e Jaco</t>
+  </si>
+  <si>
+    <t>Na epoca da Igreja Primitiva quem era a rainha da Etiopia?</t>
+  </si>
+  <si>
+    <t>Quais mulheres aparecem na lista dos herois da fe?</t>
+  </si>
+  <si>
+    <t>Quem morreu ao cair da janela enquanto o apostolo aos gentios pregava?</t>
+  </si>
+  <si>
+    <t>Jerico</t>
+  </si>
+  <si>
+    <t>Qual nome uma criança recebeu quando Israel perdeu a Gloria de Deus?</t>
+  </si>
+  <si>
+    <t>Quantos anos tinha Arao quando foi falar com Farao?</t>
+  </si>
+  <si>
+    <t>Apos orar a Deus Ezequias teve a vida prolongada por quantos anos?</t>
+  </si>
+  <si>
+    <t>Quem escreveu o livro de Atos dos Apostolos?</t>
+  </si>
+  <si>
+    <t>Qual nome da bisavo de Davi?</t>
+  </si>
+  <si>
+    <t>Golgota ou Calvario</t>
+  </si>
+  <si>
+    <t>O apostolo Paulo era natural de qual tribo de Israel?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quem recusou ser chamado de filho da filha de Farao? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quais sao os evangelhos sinoticos? </t>
+  </si>
+  <si>
+    <t>Quem reconstruiu os muros de Jerico a custa da vida de seus filhos?</t>
+  </si>
+  <si>
+    <t>Quem foi enforcado na sua propria forca?</t>
+  </si>
+  <si>
+    <t>Quantos dias levaram pra embalsamar o corpo de Jaco?</t>
+  </si>
+  <si>
+    <t>Apos a morte de Estevao quem vai para Samaria pregar o Evangelho?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quem ofereceu dinheiro aos apostolos para ter o poder de orar e as pessoas receberem o Espirito Santo? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por quantas vezes o povo de Israel rodeou a cidade de Jerico? </t>
+  </si>
+  <si>
+    <t>Jupiter e Mercurio</t>
+  </si>
+  <si>
+    <t>Qual e a unica mulher cuja idade e mencionada na Biblia?</t>
+  </si>
+  <si>
+    <t>Qual nome de um dos discipulos que iam no caminho de Emaus?</t>
+  </si>
+  <si>
+    <t>Qual parentesco de Jesus e Judas autor do penultimo livro da Biblia?</t>
+  </si>
+  <si>
+    <t>Qual rei construiu o Tunel de Siloe?</t>
+  </si>
+  <si>
+    <t>Publio</t>
+  </si>
+  <si>
+    <t>Qual era o nome da unica filha de Lia?</t>
+  </si>
+  <si>
+    <t>Nadabe e Abiu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantos anos tinha Noe quando as aguas do diluvio inundaram a terra? </t>
+  </si>
+  <si>
+    <t>A quem Paulo apelou em seu ultimo julgamento antes de ir para Roma?</t>
   </si>
 </sst>
 </file>
@@ -1636,6 +1633,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1838,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1853,7 +1854,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>64</v>
+        <v>307</v>
       </c>
       <c r="B1" s="4">
         <v>1005</v>
@@ -1863,7 +1864,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1871,59 +1872,59 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>66</v>
+        <v>424</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1</v>
+        <v>372</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>2</v>
+        <v>313</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>425</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>69</v>
+        <v>314</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>455</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>70</v>
+        <v>426</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>71</v>
+        <v>315</v>
       </c>
       <c r="B8" s="7">
         <v>2</v>
@@ -1931,109 +1932,109 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>72</v>
+        <v>373</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>73</v>
+        <v>374</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>76</v>
+        <v>277</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>278</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>12</v>
+        <v>375</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>80</v>
+        <v>274</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>15</v>
+        <v>214</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>82</v>
+        <v>215</v>
       </c>
       <c r="B19" s="5">
         <v>20</v>
@@ -2043,77 +2044,77 @@
     </row>
     <row r="20" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>83</v>
+        <v>376</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>85</v>
+        <v>456</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>86</v>
+        <v>316</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>19</v>
+        <v>309</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>87</v>
+        <v>317</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>20</v>
+        <v>427</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>88</v>
+        <v>318</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>21</v>
+        <v>319</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5">
         <v>40</v>
@@ -2123,67 +2124,67 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>93</v>
+        <v>377</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>25</v>
+        <v>320</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>94</v>
+        <v>216</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>95</v>
+        <v>378</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>96</v>
+        <v>279</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>28</v>
+        <v>217</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>97</v>
+        <v>218</v>
       </c>
       <c r="B34" s="9">
         <v>100</v>
@@ -2193,7 +2194,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>98</v>
+        <v>428</v>
       </c>
       <c r="B35" s="9">
         <v>13</v>
@@ -2203,17 +2204,17 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="B37" s="11">
         <v>39</v>
@@ -2223,527 +2224,527 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>101</v>
+        <v>280</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>102</v>
+        <v>415</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>104</v>
+        <v>275</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>105</v>
+        <v>321</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>35</v>
+        <v>281</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>107</v>
+        <v>379</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>36</v>
+        <v>322</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>108</v>
+        <v>323</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>109</v>
+        <v>219</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>38</v>
+        <v>308</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>110</v>
+        <v>429</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>39</v>
+        <v>380</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>42</v>
+        <v>324</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>113</v>
+        <v>430</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>114</v>
+        <v>431</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>44</v>
+        <v>283</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>45</v>
+        <v>325</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>116</v>
+        <v>381</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>36</v>
+        <v>322</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>134</v>
+        <v>382</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>117</v>
+        <v>326</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>118</v>
+        <v>61</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>119</v>
+        <v>327</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>50</v>
+        <v>383</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>121</v>
+        <v>432</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>122</v>
+        <v>284</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>125</v>
+        <v>328</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
-        <v>126</v>
+        <v>221</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
-        <v>128</v>
+        <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>58</v>
+        <v>222</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
-        <v>130</v>
+        <v>223</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>60</v>
+        <v>433</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
-        <v>132</v>
+        <v>310</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
-        <v>279</v>
+        <v>329</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>280</v>
+        <v>159</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>136</v>
+        <v>71</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
     <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>281</v>
+        <v>160</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>137</v>
+        <v>72</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
-        <v>283</v>
+        <v>457</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>139</v>
+        <v>74</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>284</v>
+        <v>161</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
-        <v>286</v>
+        <v>162</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>142</v>
+        <v>330</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
-        <v>287</v>
+        <v>163</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
     <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>144</v>
+        <v>286</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
-        <v>289</v>
+        <v>164</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>145</v>
+        <v>331</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
-        <v>290</v>
+        <v>384</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>146</v>
+        <v>225</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
-        <v>291</v>
+        <v>332</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>292</v>
+        <v>333</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>148</v>
+        <v>416</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
     <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>293</v>
+        <v>165</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
     <row r="88" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
-        <v>294</v>
+        <v>334</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>150</v>
+        <v>287</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
     <row r="89" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
-        <v>295</v>
+        <v>166</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>151</v>
+        <v>226</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>296</v>
+        <v>167</v>
       </c>
       <c r="B90" s="13">
         <v>100</v>
@@ -2753,87 +2754,87 @@
     </row>
     <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
-        <v>297</v>
+        <v>168</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>38</v>
+        <v>308</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
-        <v>298</v>
+        <v>385</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
-        <v>299</v>
+        <v>386</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>153</v>
+        <v>288</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
-        <v>300</v>
+        <v>227</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
     <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>155</v>
+        <v>82</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
-        <v>302</v>
+        <v>458</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>156</v>
+        <v>228</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>303</v>
+        <v>229</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>157</v>
+        <v>83</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
-        <v>304</v>
+        <v>387</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
     <row r="99" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>305</v>
+        <v>335</v>
       </c>
       <c r="B99" s="13">
         <v>40</v>
@@ -2843,17 +2844,17 @@
     </row>
     <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>159</v>
+        <v>230</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
     <row r="101" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>307</v>
+        <v>169</v>
       </c>
       <c r="B101" s="13">
         <v>8</v>
@@ -2863,37 +2864,37 @@
     </row>
     <row r="102" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
-        <v>308</v>
+        <v>388</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="18" t="s">
-        <v>309</v>
+        <v>434</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>160</v>
+        <v>85</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
     <row r="104" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>310</v>
+        <v>389</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
-        <v>311</v>
+        <v>231</v>
       </c>
       <c r="B105" s="13">
         <v>40</v>
@@ -2903,17 +2904,17 @@
     </row>
     <row r="106" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
-        <v>312</v>
+        <v>336</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
-        <v>313</v>
+        <v>337</v>
       </c>
       <c r="B107" s="13">
         <v>52</v>
@@ -2923,137 +2924,137 @@
     </row>
     <row r="108" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
-        <v>314</v>
+        <v>232</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>163</v>
+        <v>435</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
-        <v>315</v>
+        <v>436</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
-        <v>316</v>
+        <v>338</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>165</v>
+        <v>89</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
-        <v>317</v>
+        <v>437</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>166</v>
+        <v>90</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
     <row r="113" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
-        <v>319</v>
+        <v>417</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>168</v>
+        <v>92</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
     <row r="114" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
-        <v>320</v>
+        <v>170</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
-        <v>321</v>
+        <v>390</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>170</v>
+        <v>93</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>322</v>
+        <v>234</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>171</v>
+        <v>94</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
     <row r="117" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>323</v>
+        <v>391</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
     <row r="118" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>324</v>
+        <v>171</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>173</v>
+        <v>96</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
     <row r="119" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A119" s="19" t="s">
-        <v>325</v>
+        <v>172</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
     </row>
     <row r="120" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A120" s="19" t="s">
-        <v>326</v>
+        <v>235</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>174</v>
+        <v>97</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A121" s="19" t="s">
-        <v>327</v>
+        <v>173</v>
       </c>
       <c r="B121" s="13">
         <v>12</v>
@@ -3063,105 +3064,105 @@
     </row>
     <row r="122" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A122" s="19" t="s">
-        <v>328</v>
+        <v>174</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
     <row r="123" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="20" t="s">
-        <v>329</v>
+        <v>459</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>173</v>
+        <v>96</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="20" t="s">
-        <v>330</v>
+        <v>175</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>176</v>
+        <v>99</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A125" s="20" t="s">
-        <v>331</v>
+        <v>438</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>177</v>
+        <v>311</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="20" t="s">
-        <v>332</v>
+        <v>292</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>178</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="20" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>179</v>
+        <v>340</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="20" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="20" t="s">
-        <v>335</v>
+        <v>176</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>181</v>
+        <v>460</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="20" t="s">
-        <v>336</v>
+        <v>392</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A131" s="20" t="s">
-        <v>337</v>
+        <v>237</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>183</v>
+        <v>342</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="20" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>184</v>
+        <v>393</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="20" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>185</v>
+        <v>102</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A134" s="20" t="s">
-        <v>340</v>
+        <v>394</v>
       </c>
       <c r="B134" s="13">
         <v>12</v>
@@ -3169,87 +3170,87 @@
     </row>
     <row r="135" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A135" s="20" t="s">
-        <v>341</v>
+        <v>395</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>186</v>
+        <v>103</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="20" t="s">
-        <v>342</v>
+        <v>238</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>187</v>
+        <v>104</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="20" t="s">
-        <v>343</v>
+        <v>239</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>188</v>
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A138" s="20" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>189</v>
+        <v>240</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A139" s="20" t="s">
-        <v>345</v>
+        <v>293</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A140" s="20" t="s">
-        <v>346</v>
+        <v>294</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>191</v>
+        <v>107</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="20" t="s">
-        <v>347</v>
+        <v>177</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>192</v>
+        <v>295</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A142" s="20" t="s">
-        <v>348</v>
+        <v>178</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>193</v>
+        <v>108</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="20" t="s">
-        <v>349</v>
+        <v>179</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>194</v>
+        <v>241</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="20" t="s">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>195</v>
+        <v>439</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="20" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B145" s="13">
         <v>110</v>
@@ -3257,31 +3258,31 @@
     </row>
     <row r="146" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="20" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A147" s="20" t="s">
-        <v>353</v>
+        <v>440</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>197</v>
+        <v>418</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
-        <v>354</v>
+        <v>181</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A149" s="20" t="s">
-        <v>355</v>
+        <v>243</v>
       </c>
       <c r="B149" s="13">
         <v>1260</v>
@@ -3289,31 +3290,31 @@
     </row>
     <row r="150" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="20" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>199</v>
+        <v>396</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A151" s="20" t="s">
-        <v>357</v>
+        <v>397</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>200</v>
+        <v>110</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A152" s="20" t="s">
-        <v>358</v>
+        <v>398</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>201</v>
+        <v>244</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="20" t="s">
-        <v>359</v>
+        <v>441</v>
       </c>
       <c r="B153" s="13">
         <v>83</v>
@@ -3321,15 +3322,15 @@
     </row>
     <row r="154" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="20" t="s">
-        <v>360</v>
+        <v>182</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>202</v>
+        <v>111</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="20" t="s">
-        <v>361</v>
+        <v>183</v>
       </c>
       <c r="B155" s="13">
         <v>176</v>
@@ -3337,95 +3338,95 @@
     </row>
     <row r="156" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="20" t="s">
-        <v>362</v>
+        <v>461</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>44</v>
+        <v>283</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A157" s="20" t="s">
-        <v>363</v>
+        <v>184</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="20" t="s">
-        <v>364</v>
+        <v>185</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>204</v>
+        <v>112</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="20" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>205</v>
+        <v>296</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="20" t="s">
-        <v>366</v>
+        <v>186</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A161" s="20" t="s">
-        <v>367</v>
+        <v>350</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>207</v>
+        <v>246</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="20" t="s">
-        <v>368</v>
+        <v>187</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>208</v>
+        <v>114</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A163" s="20" t="s">
-        <v>369</v>
+        <v>247</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>209</v>
+        <v>115</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="20" t="s">
-        <v>370</v>
+        <v>399</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>210</v>
+        <v>116</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="20" t="s">
-        <v>371</v>
+        <v>188</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A166" s="20" t="s">
-        <v>372</v>
+        <v>248</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>212</v>
+        <v>118</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A167" s="20" t="s">
-        <v>373</v>
+        <v>442</v>
       </c>
       <c r="B167" s="13">
         <v>15</v>
@@ -3433,63 +3434,63 @@
     </row>
     <row r="168" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="20" t="s">
-        <v>374</v>
+        <v>419</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>213</v>
+        <v>119</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="20" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A170" s="20" t="s">
-        <v>376</v>
+        <v>249</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>215</v>
+        <v>297</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="20" t="s">
-        <v>377</v>
+        <v>189</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="20" t="s">
-        <v>378</v>
+        <v>190</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A173" s="20" t="s">
-        <v>379</v>
+        <v>251</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>218</v>
+        <v>120</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="20" t="s">
-        <v>380</v>
+        <v>353</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A175" s="20" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
       <c r="B175" s="13">
         <v>969</v>
@@ -3497,151 +3498,151 @@
     </row>
     <row r="176" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="20" t="s">
-        <v>382</v>
+        <v>191</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A177" s="20" t="s">
-        <v>383</v>
+        <v>300</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>221</v>
+        <v>121</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="s">
-        <v>384</v>
+        <v>192</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>222</v>
+        <v>401</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="20" t="s">
-        <v>385</v>
+        <v>193</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>223</v>
+        <v>402</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A180" s="20" t="s">
-        <v>386</v>
+        <v>301</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>224</v>
+        <v>462</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="20" t="s">
-        <v>387</v>
+        <v>354</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="20" t="s">
-        <v>388</v>
+        <v>194</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A183" s="20" t="s">
-        <v>389</v>
+        <v>355</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>227</v>
+        <v>122</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
-        <v>390</v>
+        <v>443</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A185" s="20" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A186" s="20" t="s">
-        <v>392</v>
+        <v>255</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>230</v>
+        <v>356</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="20" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="20" t="s">
-        <v>394</v>
+        <v>444</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>232</v>
+        <v>126</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="s">
-        <v>395</v>
+        <v>302</v>
       </c>
       <c r="B189" s="13">
         <v>400</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B190" s="13" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A191" s="20" t="s">
-        <v>396</v>
+        <v>357</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A192" s="20" t="s">
-        <v>397</v>
+        <v>195</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>235</v>
+        <v>303</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193" s="20" t="s">
-        <v>398</v>
+        <v>196</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>236</v>
+        <v>445</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="20" t="s">
-        <v>399</v>
+        <v>358</v>
       </c>
       <c r="B194" s="13">
         <v>2</v>
@@ -3649,55 +3650,55 @@
     </row>
     <row r="195" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A195" s="20" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="s">
-        <v>401</v>
+        <v>256</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>238</v>
+        <v>129</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="20" t="s">
-        <v>402</v>
+        <v>446</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>239</v>
+        <v>130</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="20" t="s">
-        <v>403</v>
+        <v>257</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>240</v>
+        <v>359</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="20" t="s">
-        <v>404</v>
+        <v>447</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>36</v>
+        <v>322</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="20" t="s">
-        <v>405</v>
+        <v>448</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>241</v>
+        <v>131</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A201" s="20" t="s">
-        <v>406</v>
+        <v>463</v>
       </c>
       <c r="B201" s="13">
         <v>600</v>
@@ -3705,63 +3706,63 @@
     </row>
     <row r="202" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
-        <v>407</v>
+        <v>360</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>242</v>
+        <v>132</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="20" t="s">
-        <v>408</v>
+        <v>361</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A204" s="20" t="s">
-        <v>409</v>
+        <v>197</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>244</v>
+        <v>134</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A205" s="20" t="s">
-        <v>410</v>
+        <v>362</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>245</v>
+        <v>135</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="20" t="s">
-        <v>411</v>
+        <v>258</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A207" s="20" t="s">
-        <v>412</v>
+        <v>464</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>246</v>
+        <v>363</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="s">
-        <v>413</v>
+        <v>198</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>247</v>
+        <v>136</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A209" s="20" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="B209" s="13">
         <v>60</v>
@@ -3769,79 +3770,79 @@
     </row>
     <row r="210" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="20" t="s">
-        <v>415</v>
+        <v>199</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>248</v>
+        <v>137</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A211" s="20" t="s">
-        <v>416</v>
+        <v>200</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="20" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="B212" s="13" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213" s="20" t="s">
-        <v>418</v>
+        <v>201</v>
       </c>
       <c r="B213" s="13" t="s">
-        <v>250</v>
+        <v>138</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
-        <v>419</v>
+        <v>202</v>
       </c>
       <c r="B214" s="13" t="s">
-        <v>251</v>
+        <v>139</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215" s="20" t="s">
-        <v>420</v>
+        <v>304</v>
       </c>
       <c r="B215" s="13" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="20" t="s">
-        <v>421</v>
+        <v>364</v>
       </c>
       <c r="B216" s="13" t="s">
-        <v>253</v>
+        <v>140</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A217" s="20" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="B217" s="13" t="s">
-        <v>254</v>
+        <v>141</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218" s="20" t="s">
-        <v>423</v>
+        <v>260</v>
       </c>
       <c r="B218" s="13" t="s">
-        <v>255</v>
+        <v>142</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219" s="20" t="s">
-        <v>424</v>
+        <v>365</v>
       </c>
       <c r="B219" s="13">
         <v>20</v>
@@ -3849,7 +3850,7 @@
     </row>
     <row r="220" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
-        <v>425</v>
+        <v>203</v>
       </c>
       <c r="B220" s="13">
         <v>42</v>
@@ -3857,39 +3858,39 @@
     </row>
     <row r="221" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221" s="20" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>36</v>
+        <v>322</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A222" s="20" t="s">
-        <v>427</v>
+        <v>449</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>256</v>
+        <v>143</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="20" t="s">
-        <v>428</v>
+        <v>204</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>257</v>
+        <v>144</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224" s="20" t="s">
-        <v>429</v>
+        <v>450</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
-        <v>430</v>
+        <v>451</v>
       </c>
       <c r="B225" s="13">
         <v>40</v>
@@ -3897,63 +3898,63 @@
     </row>
     <row r="226" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A226" s="20" t="s">
-        <v>431</v>
+        <v>452</v>
       </c>
       <c r="B226" s="13" t="s">
-        <v>259</v>
+        <v>145</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A227" s="20" t="s">
-        <v>432</v>
+        <v>262</v>
       </c>
       <c r="B227" s="13" t="s">
-        <v>260</v>
+        <v>146</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A228" s="20" t="s">
-        <v>433</v>
+        <v>453</v>
       </c>
       <c r="B228" s="13" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
-        <v>434</v>
+        <v>205</v>
       </c>
       <c r="B229" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A230" s="20" t="s">
-        <v>435</v>
+        <v>409</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>263</v>
+        <v>148</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231" s="20" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>264</v>
+        <v>149</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="20" t="s">
-        <v>437</v>
+        <v>312</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>265</v>
+        <v>150</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
-        <v>438</v>
+        <v>366</v>
       </c>
       <c r="B233" s="13">
         <v>85</v>
@@ -3961,7 +3962,7 @@
     </row>
     <row r="234" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234" s="20" t="s">
-        <v>439</v>
+        <v>410</v>
       </c>
       <c r="B234" s="13">
         <v>3</v>
@@ -3969,23 +3970,23 @@
     </row>
     <row r="235" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A235" s="20" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>266</v>
+        <v>151</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A236" s="20" t="s">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="B236" s="13" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
-        <v>442</v>
+        <v>264</v>
       </c>
       <c r="B237" s="13">
         <v>930</v>
@@ -3993,7 +3994,7 @@
     </row>
     <row r="238" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238" s="20" t="s">
-        <v>443</v>
+        <v>412</v>
       </c>
       <c r="B238" s="13">
         <v>260</v>
@@ -4001,31 +4002,31 @@
     </row>
     <row r="239" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239" s="20" t="s">
-        <v>444</v>
+        <v>206</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="20" t="s">
-        <v>445</v>
+        <v>266</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A241" s="20" t="s">
-        <v>446</v>
+        <v>207</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A242" s="20" t="s">
-        <v>447</v>
+        <v>413</v>
       </c>
       <c r="B242" s="13">
         <v>70</v>
@@ -4033,79 +4034,79 @@
     </row>
     <row r="243" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A243" s="20" t="s">
-        <v>448</v>
+        <v>208</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>270</v>
+        <v>305</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="20" t="s">
-        <v>449</v>
+        <v>306</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>145</v>
+        <v>331</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A245" s="20" t="s">
-        <v>450</v>
+        <v>367</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>271</v>
+        <v>154</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A246" s="20" t="s">
-        <v>451</v>
+        <v>368</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>4</v>
+        <v>455</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A247" s="20" t="s">
-        <v>452</v>
+        <v>209</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A248" s="20" t="s">
-        <v>453</v>
+        <v>414</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>178</v>
+        <v>100</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A249" s="20" t="s">
-        <v>454</v>
+        <v>210</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A250" s="20" t="s">
-        <v>455</v>
+        <v>369</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>273</v>
+        <v>370</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="20" t="s">
-        <v>456</v>
+        <v>268</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>274</v>
+        <v>155</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A252" s="20" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B252" s="13">
         <v>13</v>
@@ -4113,31 +4114,31 @@
     </row>
     <row r="253" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253" s="20" t="s">
-        <v>458</v>
+        <v>269</v>
       </c>
       <c r="B253" s="13" t="s">
-        <v>177</v>
+        <v>311</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A254" s="20" t="s">
-        <v>459</v>
+        <v>211</v>
       </c>
       <c r="B254" s="13" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A255" s="20" t="s">
-        <v>460</v>
+        <v>270</v>
       </c>
       <c r="B255" s="13" t="s">
-        <v>275</v>
+        <v>156</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A256" s="20" t="s">
-        <v>461</v>
+        <v>371</v>
       </c>
       <c r="B256" s="13">
         <v>18</v>
@@ -4145,34 +4146,34 @@
     </row>
     <row r="257" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A257" s="20" t="s">
-        <v>462</v>
+        <v>212</v>
       </c>
       <c r="B257" s="13" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A258" s="20" t="s">
-        <v>463</v>
+        <v>272</v>
       </c>
       <c r="B258" s="13" t="s">
-        <v>277</v>
+        <v>157</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A259" s="20" t="s">
-        <v>464</v>
+        <v>273</v>
       </c>
       <c r="B259" s="13" t="s">
-        <v>278</v>
+        <v>158</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A260" s="20" t="s">
-        <v>465</v>
+        <v>213</v>
       </c>
       <c r="B260" s="13" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>